<commit_message>
Ensure cop22OPU_data_pack_schema is created correctly from unPackSchema
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_OPU_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_OPU_Data_Pack_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://guidehouse-my.sharepoint.us/personal/cnemarich_guidehousefederal_com/Documents/Documents/GitHub/datapackr/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{7E6314B4-AC33-2D4A-AF0A-1BE11FAD4A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F816873A-2E31-41E5-B9D6-EF5FE776B2BB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387AEBA-54D9-BB47-AA2C-1750F201DB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PSNUxIM!$A$14:$AK$16</definedName>
     <definedName name="MIN_DSD" localSheetId="1">ROUND(MAX(IF(ISNUMBER(FIND("DSD",PSNUxIM!$CW$14:$FS$14)),PSNUxIM!$CW1:$FS1)),1)</definedName>
-    <definedName name="MIN_DSD">ROUND(MAX(IF(ISNUMBER(FIND("DSD",PSNUxIM!$CW$14:$FS$14)),PSNUxIM!$CW1:$FS1)),1)</definedName>
     <definedName name="MIN_TA" localSheetId="1">ROUND(MAX(IF(ISNUMBER(FIND("TA",PSNUxIM!$CW$14:$FS$14)),PSNUxIM!$CW1:$FS1)),1)</definedName>
-    <definedName name="MIN_TA">ROUND(MAX(IF(ISNUMBER(FIND("TA",#REF!)),#REF!)),1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1123,27 +1121,27 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="46" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" ht="47" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="97" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:2" ht="97" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="81.5" x14ac:dyDescent="1.75">
+    <row r="20" spans="2:2" ht="82" x14ac:dyDescent="0.9">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1161,11 +1159,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B207F3C7-F002-E540-88C1-75A9C9657E34}">
   <dimension ref="A1:FS23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CX9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DN15" sqref="DN15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.83203125" customWidth="1"/>
@@ -1190,7 +1188,7 @@
     <col min="101" max="175" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:175" ht="31" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:175" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>20</v>
       </c>
@@ -1375,7 +1373,7 @@
       <c r="FR1" s="8"/>
       <c r="FS1" s="8"/>
     </row>
-    <row r="2" spans="1:175" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:175" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="24"/>
@@ -1564,7 +1562,7 @@
       <c r="FR2" s="6"/>
       <c r="FS2" s="6"/>
     </row>
-    <row r="3" spans="1:175" ht="118" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:175" ht="118" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="78" t="s">
         <v>29</v>
       </c>
@@ -1755,7 +1753,7 @@
       <c r="FR3" s="6"/>
       <c r="FS3" s="6"/>
     </row>
-    <row r="4" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1932,7 +1930,7 @@
       <c r="FR4" s="15"/>
       <c r="FS4" s="15"/>
     </row>
-    <row r="5" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A5" s="44" t="s">
         <v>11</v>
       </c>
@@ -2459,7 +2457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
         <v>15</v>
       </c>
@@ -2986,7 +2984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A7" s="44" t="s">
         <v>12</v>
       </c>
@@ -3513,7 +3511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A8" s="44" t="s">
         <v>33</v>
       </c>
@@ -4040,7 +4038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A9" s="44" t="s">
         <v>33</v>
       </c>
@@ -4567,7 +4565,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A10" s="44" t="s">
         <v>33</v>
       </c>
@@ -5094,7 +5092,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A11" s="44" t="s">
         <v>33</v>
       </c>
@@ -5621,7 +5619,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
         <v>33</v>
       </c>
@@ -6148,7 +6146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
         <v>33</v>
       </c>
@@ -6675,7 +6673,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:175" ht="117" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:175" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="58" t="s">
         <v>0</v>
       </c>
@@ -7131,7 +7129,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:175" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -7572,7 +7570,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:175" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:175" x14ac:dyDescent="0.2">
       <c r="H16" s="43"/>
       <c r="CF16" s="12"/>
       <c r="CG16" s="12"/>
@@ -7597,7 +7595,7 @@
       <c r="CZ16" s="15"/>
       <c r="DA16" s="15"/>
     </row>
-    <row r="17" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H17" s="43"/>
       <c r="CF17" s="12"/>
       <c r="CG17" s="12"/>
@@ -7622,7 +7620,7 @@
       <c r="CZ17" s="15"/>
       <c r="DA17" s="15"/>
     </row>
-    <row r="18" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H18" s="43"/>
       <c r="CF18" s="12"/>
       <c r="CG18" s="12"/>
@@ -7647,7 +7645,7 @@
       <c r="CZ18" s="15"/>
       <c r="DA18" s="15"/>
     </row>
-    <row r="19" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H19" s="43"/>
       <c r="CF19" s="12"/>
       <c r="CG19" s="12"/>
@@ -7672,7 +7670,7 @@
       <c r="CZ19" s="15"/>
       <c r="DA19" s="15"/>
     </row>
-    <row r="20" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H20" s="43"/>
       <c r="CF20" s="12"/>
       <c r="CG20" s="12"/>
@@ -7697,7 +7695,7 @@
       <c r="CZ20" s="15"/>
       <c r="DA20" s="15"/>
     </row>
-    <row r="21" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H21" s="43"/>
       <c r="CF21" s="12"/>
       <c r="CG21" s="12"/>
@@ -7722,7 +7720,7 @@
       <c r="CZ21" s="15"/>
       <c r="DA21" s="15"/>
     </row>
-    <row r="22" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H22" s="43"/>
       <c r="CF22" s="12"/>
       <c r="CG22" s="12"/>
@@ -7747,7 +7745,7 @@
       <c r="CZ22" s="15"/>
       <c r="DA22" s="15"/>
     </row>
-    <row r="23" spans="8:105" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:105" x14ac:dyDescent="0.2">
       <c r="H23" s="43"/>
       <c r="CF23" s="12"/>
       <c r="CG23" s="12"/>

</xml_diff>

<commit_message>
Fix issues causing dropping of dedupes.
- Only changes to template and schema are to fix extra spaces in Custom DSD and Crosswalk Dedupe Allocation column names.
- Remove superfluous notes not related to explaining coding choices.
- Add TODOs where needs speeding up
</commit_message>
<xml_diff>
--- a/inst/extdata/COP22_OPU_Data_Pack_Template.xlsx
+++ b/inst/extdata/COP22_OPU_Data_Pack_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott/Documents/GitHub/datapackr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2387AEBA-54D9-BB47-AA2C-1750F201DB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F9BA6A-38D8-864D-B643-3EB9F8A7B5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{6350F473-330A-BA43-B59F-2231AEF8C02D}"/>
   </bookViews>
@@ -205,16 +205,10 @@
     <t>Crosswalk Dedupe Resolution</t>
   </si>
   <si>
-    <t>Custom Crosswalk Dedupe Allocation  (% of DataPackTarget)</t>
-  </si>
-  <si>
     <t>Total Deduplicated Rollup</t>
   </si>
   <si>
     <t>DSD Dedupe Resolution</t>
-  </si>
-  <si>
-    <t>Custom DSD Dedupe Allocation  (% of DataPackTarget)</t>
   </si>
   <si>
     <t>Deduplicated DSD Rollup</t>
@@ -227,6 +221,12 @@
   </si>
   <si>
     <t>TA Dedupe Resolution</t>
+  </si>
+  <si>
+    <t>Custom DSD Dedupe Allocation (% of DataPackTarget)</t>
+  </si>
+  <si>
+    <t>Custom Crosswalk Dedupe Allocation (% of DataPackTarget)</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B207F3C7-F002-E540-88C1-75A9C9657E34}">
   <dimension ref="A1:FS23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="CG1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI15" sqref="CI15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6787,10 +6787,10 @@
         <v>46</v>
       </c>
       <c r="CI14" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="CJ14" s="69" t="s">
         <v>47</v>
-      </c>
-      <c r="CJ14" s="69" t="s">
-        <v>48</v>
       </c>
       <c r="CK14" s="13" t="s">
         <v>39</v>
@@ -6802,13 +6802,13 @@
         <v>41</v>
       </c>
       <c r="CN14" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="CO14" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="CP14" s="69" t="s">
         <v>49</v>
-      </c>
-      <c r="CO14" s="68" t="s">
-        <v>50</v>
-      </c>
-      <c r="CP14" s="69" t="s">
-        <v>51</v>
       </c>
       <c r="CQ14" s="13" t="s">
         <v>42</v>
@@ -6820,13 +6820,13 @@
         <v>44</v>
       </c>
       <c r="CT14" s="67" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="CU14" s="68" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="CV14" s="69" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="CW14" s="70" t="str">
         <f t="shared" ref="CW14:FH14" si="0">IF(I14="","",I$14)</f>

</xml_diff>